<commit_message>
Risks analysis fixed version
</commit_message>
<xml_diff>
--- a/docs/Аналіз_ризиків.xlsx
+++ b/docs/Аналіз_ризиків.xlsx
@@ -219,103 +219,103 @@
     <t>Program Constraints / Resources / Staff</t>
   </si>
   <si>
+    <t>Identified</t>
+  </si>
+  <si>
+    <t>Відсутність робочої взаємодії із замовником</t>
+  </si>
+  <si>
+    <t>Використовувати спільні платформи та інструменти, забезпечувати своєчасне інформування замовника про стан проекту, визначати конкретних відповідальних осіб у команді розробників та в замовника для забезпечення чіткої комунікації</t>
+  </si>
+  <si>
+    <t>Development Environment / Work Environment / Communication</t>
+  </si>
+  <si>
+    <t>Невизначеність вимог замовника</t>
+  </si>
+  <si>
+    <t>Регулярна комунікація з замовником, розробка детального технічного завдання</t>
+  </si>
+  <si>
+    <t xml:space="preserve">активні бойові дії </t>
+  </si>
+  <si>
+    <t>Музичина. А</t>
+  </si>
+  <si>
+    <t>Мати запас часу</t>
+  </si>
+  <si>
+    <t>Program Constraints / Other</t>
+  </si>
+  <si>
+    <t>Впав сервер</t>
+  </si>
+  <si>
+    <t>Acceptance</t>
+  </si>
+  <si>
+    <t>Моніторинг сервера</t>
+  </si>
+  <si>
+    <t>Development Environment / Development System / Reliability</t>
+  </si>
+  <si>
+    <t>Впав веб-сервер</t>
+  </si>
+  <si>
+    <t>Чорноморець М.</t>
+  </si>
+  <si>
+    <t>Використання багатопотокової архітектури, моніторинг сервера, використання балансувальників навантаження</t>
+  </si>
+  <si>
+    <t>Взлом сервера</t>
+  </si>
+  <si>
+    <t>Пащенко М.</t>
+  </si>
+  <si>
+    <t>Моніторинг сервера, Регулярне оновлення програмного забезпечення, Використання багатофакторної аутентифікації, Резервне копіювання даних.</t>
+  </si>
+  <si>
+    <t>Product Engineering / Engineering Specialties / Security</t>
+  </si>
+  <si>
+    <t>відключення електроенергії</t>
+  </si>
+  <si>
+    <t>Андресюк Д.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Помилка розробників </t>
+  </si>
+  <si>
+    <t>Навчання розробників,код-рев'ю, тестування, автоматизація процесів розробки</t>
+  </si>
+  <si>
+    <t>Product Engineering / Engineering Specialties / Human Factors</t>
+  </si>
+  <si>
+    <t>Analyzed</t>
+  </si>
+  <si>
+    <t>Пандемія</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Впала база даних </t>
+  </si>
+  <si>
+    <t>Моніторинг бази даних та створення резервної копії даних</t>
+  </si>
+  <si>
     <t>Розростання обсягу проекту</t>
   </si>
   <si>
-    <t>Пащенко М.</t>
-  </si>
-  <si>
     <t>Зафіксувати об'єм проекту шляхом створення чітких параметрів для нього</t>
   </si>
   <si>
     <t>Program Constraints / Resources / Facilities</t>
-  </si>
-  <si>
-    <t>Analyzed</t>
-  </si>
-  <si>
-    <t>Пандемія</t>
-  </si>
-  <si>
-    <t>Acceptance</t>
-  </si>
-  <si>
-    <t>Чорноморець М.</t>
-  </si>
-  <si>
-    <t>Program Constraints / Other</t>
-  </si>
-  <si>
-    <t>Identified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">активні бойові дії </t>
-  </si>
-  <si>
-    <t>Музичина. А</t>
-  </si>
-  <si>
-    <t>Мати запас часу</t>
-  </si>
-  <si>
-    <t>відключення електроенергії</t>
-  </si>
-  <si>
-    <t>Андресюк Д.</t>
-  </si>
-  <si>
-    <t>Відсутність робочої взаємодії із замовником</t>
-  </si>
-  <si>
-    <t>Використовувати спільні платформи та інструменти, забезпечувати своєчасне інформування замовника про стан проекту, визначати конкретних відповідальних осіб у команді розробників та в замовника для забезпечення чіткої комунікації</t>
-  </si>
-  <si>
-    <t>Development Environment / Work Environment / Communication</t>
-  </si>
-  <si>
-    <t>Невизначеність вимог замовника</t>
-  </si>
-  <si>
-    <t>Регулярна комунікація з замовником, розробка детального технічного завдання</t>
-  </si>
-  <si>
-    <t>Впав сервер</t>
-  </si>
-  <si>
-    <t>Моніторинг сервера</t>
-  </si>
-  <si>
-    <t>Development Environment / Development System / Reliability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Впала база даних </t>
-  </si>
-  <si>
-    <t>Моніторинг бази даних та створення резервної копії даних</t>
-  </si>
-  <si>
-    <t>Впав веб-сервер</t>
-  </si>
-  <si>
-    <t>Використання багатопотокової архітектури, моніторинг сервера, використання балансувальників навантаження</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Помилка розробників </t>
-  </si>
-  <si>
-    <t>Навчання розробників,код-рев'ю, тестування, автоматизація процесів розробки</t>
-  </si>
-  <si>
-    <t>Product Engineering / Engineering Specialties / Human Factors</t>
-  </si>
-  <si>
-    <t>Взлом сервера</t>
-  </si>
-  <si>
-    <t>Моніторинг сервера, Регулярне оновлення програмного забезпечення, Використання багатофакторної аутентифікації, Резервне копіювання даних.</t>
-  </si>
-  <si>
-    <t>Product Engineering / Engineering Specialties / Security</t>
   </si>
   <si>
     <t>Impact Scale</t>
@@ -745,8 +745,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;&quot;р.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_р_._-;\-* #,##0_р_._-;_-* &quot;-&quot;_р_._-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_р_._-;\-* #,##0_р_._-;_-* &quot;-&quot;_р_._-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -809,8 +809,89 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="36"/>
+      <name val="Arial"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -824,8 +905,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -839,105 +936,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <charset val="204"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="36"/>
-      <name val="Arial"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -974,7 +974,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -986,7 +992,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,163 +1154,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1231,35 +1231,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1293,23 +1264,26 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399975585192419"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1331,70 +1305,96 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
+      <bottom style="thick">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1876,8 +1876,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="13"/>
@@ -1886,9 +1886,9 @@
     <col min="2" max="2" width="7.55454545454545" style="19"/>
     <col min="3" max="3" width="29.7272727272727" customWidth="1"/>
     <col min="4" max="4" width="10.8909090909091" style="20" customWidth="1"/>
-    <col min="5" max="6" width="4.55454545454545" style="20"/>
+    <col min="5" max="6" width="4.57272727272727" style="20"/>
     <col min="7" max="7" width="5.44545454545455" style="21" customWidth="1"/>
-    <col min="8" max="8" width="10.1090909090909" style="20"/>
+    <col min="8" max="8" width="15.3363636363636" style="20" customWidth="1"/>
     <col min="9" max="9" width="9.10909090909091" style="20" customWidth="1"/>
     <col min="10" max="10" width="36.2909090909091" style="18" customWidth="1"/>
     <col min="11" max="11" width="27.2727272727273" customWidth="1"/>
@@ -1948,11 +1948,11 @@
         <v>0.4</v>
       </c>
       <c r="F2" s="27">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G2" s="28">
-        <f t="shared" ref="G2:G9" si="0">$E2*$F2</f>
-        <v>0.32</v>
+        <f t="shared" ref="G2:G16" si="0">$E2*$F2</f>
+        <v>0.36</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>15</v>
@@ -1985,11 +1985,11 @@
         <v>0.4</v>
       </c>
       <c r="F3" s="27">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G3" s="28">
         <f t="shared" si="0"/>
-        <v>0.32</v>
+        <v>0.28</v>
       </c>
       <c r="H3" s="26" t="s">
         <v>21</v>
@@ -2010,29 +2010,29 @@
     <row r="4" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A4" s="24"/>
       <c r="B4" s="25" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="27">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="F4" s="27">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="G4" s="28">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.28</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I4" s="26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J4" s="24" t="s">
         <v>26</v>
@@ -2047,47 +2047,47 @@
     <row r="5" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A5" s="24"/>
       <c r="B5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>29</v>
-      </c>
       <c r="D5" s="26" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E5" s="27">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="F5" s="27">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="G5" s="28">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.28</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I5" s="26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="K5" s="24" t="s">
         <v>17</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A6" s="24"/>
       <c r="B6" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>14</v>
@@ -2096,54 +2096,54 @@
         <v>0.8</v>
       </c>
       <c r="F6" s="27">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="G6" s="28">
         <f t="shared" si="0"/>
-        <v>0.32</v>
+        <v>0.24</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I6" s="26">
         <v>300</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K6" s="24" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A7" s="24"/>
       <c r="B7" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E7" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="27">
         <v>0.1</v>
       </c>
-      <c r="F7" s="27">
-        <v>0.8</v>
-      </c>
       <c r="G7" s="28">
-        <f t="shared" si="0"/>
+        <f>$E7*$F7</f>
         <v>0.08</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I7" s="26">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="J7" s="24" t="s">
         <v>36</v>
@@ -2152,35 +2152,35 @@
         <v>17</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A8" s="24"/>
       <c r="B8" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="27">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="F8" s="27">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="G8" s="28">
-        <f t="shared" si="0"/>
-        <v>0.32</v>
+        <f>$E8*$F8</f>
+        <v>0.08</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="I8" s="26">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J8" s="24" t="s">
         <v>40</v>
@@ -2189,35 +2189,35 @@
         <v>17</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A9" s="24"/>
       <c r="B9" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C9" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="28">
+        <f>$E9*$F9</f>
+        <v>0.08</v>
+      </c>
+      <c r="H9" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="27">
-        <v>0.4</v>
-      </c>
-      <c r="F9" s="27">
-        <v>0.8</v>
-      </c>
-      <c r="G9" s="28">
-        <f t="shared" si="0"/>
-        <v>0.32</v>
-      </c>
-      <c r="H9" s="26" t="s">
-        <v>21</v>
-      </c>
       <c r="I9" s="26">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="J9" s="24" t="s">
         <v>43</v>
@@ -2226,50 +2226,50 @@
         <v>17</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A10" s="24"/>
       <c r="B10" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E10" s="27">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="F10" s="27">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="G10" s="28">
-        <f t="shared" ref="G10:G16" si="1">$E10*$F10</f>
-        <v>0.08</v>
+        <f>$E10*$F10</f>
+        <v>0.07</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="I10" s="26">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="K10" s="24" t="s">
         <v>17</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A11" s="24"/>
       <c r="B11" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>47</v>
@@ -2278,20 +2278,20 @@
         <v>14</v>
       </c>
       <c r="E11" s="27">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="F11" s="27">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G11" s="28">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
+        <f>$E11*$F11</f>
+        <v>0.06</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I11" s="26">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="J11" s="24" t="s">
         <v>48</v>
@@ -2300,109 +2300,109 @@
         <v>17</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A12" s="24"/>
       <c r="B12" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E12" s="27">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="F12" s="27">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G12" s="28">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
+        <f>$E12*$F12</f>
+        <v>0.03</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="I12" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="K12" s="24" t="s">
         <v>17</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A13" s="24"/>
       <c r="B13" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="27">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F13" s="27">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G13" s="28">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
+        <f>$E13*$F13</f>
+        <v>0.02</v>
       </c>
       <c r="H13" s="26" t="s">
         <v>31</v>
       </c>
       <c r="I13" s="26">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K13" s="24" t="s">
         <v>17</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" s="15" customFormat="1" ht="10" spans="1:12">
       <c r="A14" s="24"/>
       <c r="B14" s="25" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>54</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E14" s="27">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="F14" s="27">
         <v>0.1</v>
       </c>
       <c r="G14" s="28">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
+        <f t="shared" si="0"/>
+        <v>0.01</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="I14" s="26">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J14" s="24" t="s">
         <v>55</v>
@@ -2414,39 +2414,31 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" s="15" customFormat="1" ht="10" spans="1:12">
+    <row r="15" s="15" customFormat="1" ht="10" spans="1:11">
       <c r="A15" s="24"/>
       <c r="B15" s="25"/>
       <c r="C15" s="24"/>
       <c r="D15" s="26"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
-      <c r="G15" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G15" s="26"/>
       <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-    </row>
-    <row r="16" s="15" customFormat="1" ht="10" spans="1:12">
+    </row>
+    <row r="16" s="15" customFormat="1" ht="10" spans="1:11">
       <c r="A16" s="24"/>
       <c r="B16" s="25"/>
       <c r="C16" s="24"/>
       <c r="D16" s="26"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
-      <c r="G16" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="G16" s="26"/>
       <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="24"/>
       <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
     </row>
     <row r="17" s="15" customFormat="1" ht="10.5" spans="1:12">
       <c r="A17" s="30"/>
@@ -5058,6 +5050,9 @@
       <c r="F226" s="42"/>
     </row>
   </sheetData>
+  <sortState ref="A2:L16">
+    <sortCondition ref="G2" descending="1"/>
+  </sortState>
   <conditionalFormatting sqref="B1:B65530">
     <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>"Occurred"</formula>
@@ -5069,7 +5064,7 @@
       <formula>"Analyzed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G65530">
+  <conditionalFormatting sqref="G1:G14;G17:G65530">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="between">
       <formula>0.001</formula>
       <formula>0.05</formula>
@@ -5084,10 +5079,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2:L4;L5:L7;L8:L9;L10:L65530">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K15:K16;L2:L4;L5:L7;L8:L9;L10:L14;L17:L65530">
       <formula1>Domain</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E4;E5:E7;E8:E9;E10:E65530;F2:F4;F5:F7;F8:F9;F10:F14">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E4;E5:E7;E8:E9;E10:E65530">
       <formula1>ImpactScale</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B4;B5:B7;B8:B9;B10:B65530">
@@ -5096,7 +5091,7 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D4;D5:D7;D8:D9;D10:D65530">
       <formula1>MitigationStrategy</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F15:F65530">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F14;F15:F65530">
       <formula1>ProbabilityScale</formula1>
     </dataValidation>
   </dataValidations>
@@ -5113,7 +5108,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" zoomScaleSheetLayoutView="60" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -5198,7 +5193,7 @@
         <v>65</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5206,10 +5201,10 @@
         <v>66</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>12</v>
@@ -5444,7 +5439,7 @@
         <v>117</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5452,7 +5447,7 @@
         <v>118</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -5548,7 +5543,7 @@
         <v>141</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5652,7 +5647,7 @@
         <v>166</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -5700,7 +5695,7 @@
         <v>175</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -5788,7 +5783,7 @@
         <v>196</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>